<commit_message>
Tentativa de por a funcionar o motor do excel
</commit_message>
<xml_diff>
--- a/Analisador/test.xlsx
+++ b/Analisador/test.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunocarvalho/Documents/LEI/Analisador/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A36C5DB-A76C-0149-AED5-4BA31CE141EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Estatistica" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Prejudice</t>
   </si>
@@ -64,6 +58,9 @@
     <t>UgzjNcg_wbFCVXy0_qd4AaABAg</t>
   </si>
   <si>
+    <t>[('Puta', 1, 30)]</t>
+  </si>
+  <si>
     <t>O que eu constato de tudo isto é que essa Câncio é burra que nem uma porta, além de inculta: então namorou com ele, viveu em hoteis de luxo com ele, via a vida carissíma que ele levava e não desconfiou de nada? Nadinha de nada?! Isso só se tem algum atraso mental porque qualquer pessoa medianamente dotada " via logo o filme todo".... Ela com tanta falta de " percebes", fez o 12 ano e tirou o curso, como?! Saiu-lhe o diploma na Farinha Amparo?!</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
     <t>UgyPLVoPyjwDRBac_4J4AaABAg</t>
   </si>
   <si>
+    <t>[('Puta', 1, 15)]</t>
+  </si>
+  <si>
     <t>Ugzm6d-Zi5AFab6xNZ54AaABAg</t>
   </si>
   <si>
@@ -127,47 +127,87 @@
     <t>[('Vaca', 1, 10)]</t>
   </si>
   <si>
+    <t>Racism</t>
+  </si>
+  <si>
+    <t>E lamentavel as sanguessugas que chupam a veia da nossa pátria. Sem ofensa (E um gajo aqui a tentar sobreviver com a miséria do ordenado mínimo) ate o bruno de carvalho tem mais visualizações a dar um peido nas antas. Como lavam os olhos com futebol e novelas.</t>
+  </si>
+  <si>
+    <t>Ugz2i79bEUTSPrjxLoF4AaABAg</t>
+  </si>
+  <si>
+    <t>[('Gajo', 1, 48)]</t>
+  </si>
+  <si>
+    <t>Classism</t>
+  </si>
+  <si>
+    <t>Pelos vistos ninguém aqui foi inquirido em nenhum processo.... sim o ministério publico tem o habito de mandar à parede para ver se cola. A melhor defesa é o ataque! Se querem respostas façam perguntas concretas. Assim se evita de se auto-incriminar. Principalmente num processo como este, julgamentos públicos, provas que muitas vezes não passam de indícios... Lamento, quando não tenho absolutamente nada a ser recriminado também vou ao ataque... sim já me tentaram acusar de crimes que não cometi, por isso hoje até num qualquer controlo de trânsito vou ao ataque. 
+Assim de repente... não sei em que ano fui a Veneza, a Santorini, à R. Dominicana, à Jamaica..... Teria de pensar bem nas férias para poder ter a certeza em que ano foi. Sei lá... oh estava na Grand Canária em janeiro de 2002. Porque sei? Lembro-me do problema que foi a chegada de Alemães com notas de 500€! Em julho de 98 estava na R. Dominicana, lembro-me de conhecer 2 franceses super excitados com o mundial.   Mas se me perguntarem de repente quando foi uma destas viagens... ficaria um pouco à rasca para me lembrar do ano, teria de pensar nestes pequenos detalhes para me lembrar do ano... se existirem detalhes que o permitam.</t>
+  </si>
+  <si>
+    <t>UgxRqe__MPAHjzTe9nJ4AaABAg</t>
+  </si>
+  <si>
+    <t>[('Rasca', 1, 207)]</t>
+  </si>
+  <si>
+    <t>Intolerance_to</t>
+  </si>
+  <si>
+    <t>Ó Sra. Doutora Psicologa eu não gosto de levar no rabo, sou homofóbico?</t>
+  </si>
+  <si>
+    <t>UgzQHJ4RbzDOCwkBIo54AaABAg</t>
+  </si>
+  <si>
+    <t>[('homofóbico', 1, 13)]</t>
+  </si>
+  <si>
     <t>Ocorrencias</t>
   </si>
   <si>
-    <t>Gaja ----&gt; 2</t>
-  </si>
-  <si>
-    <t>Loira ----&gt; 1</t>
-  </si>
-  <si>
-    <t>Cabra ----&gt; 2</t>
-  </si>
-  <si>
-    <t>Burra ----&gt; 3</t>
-  </si>
-  <si>
-    <t>Vaca ----&gt; 2</t>
-  </si>
-  <si>
-    <t>Puta ----&gt; 3</t>
-  </si>
-  <si>
-    <t>Feiosa ----&gt; 1</t>
-  </si>
-  <si>
-    <t>Ordinária ----&gt; 1</t>
-  </si>
-  <si>
-    <t>11/42</t>
-  </si>
-  <si>
-    <t>[('P*ta', 1, 30)]</t>
-  </si>
-  <si>
-    <t>[('P*ta', 1, 15)]</t>
+    <t>Feiosa ----&gt; 2</t>
+  </si>
+  <si>
+    <t>Burra ----&gt; 6</t>
+  </si>
+  <si>
+    <t>Gajo ----&gt; 1</t>
+  </si>
+  <si>
+    <t>Ordinária ----&gt; 2</t>
+  </si>
+  <si>
+    <t>Vaca ----&gt; 4</t>
+  </si>
+  <si>
+    <t>Gaja ----&gt; 4</t>
+  </si>
+  <si>
+    <t>homofóbico ----&gt; 1</t>
+  </si>
+  <si>
+    <t>Cabra ----&gt; 4</t>
+  </si>
+  <si>
+    <t>Puta ----&gt; 6</t>
+  </si>
+  <si>
+    <t>Rasca ----&gt; 1</t>
+  </si>
+  <si>
+    <t>Loira ----&gt; 2</t>
+  </si>
+  <si>
+    <t>25/42</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,16 +217,16 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,29 +267,21 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -291,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,27 +355,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,24 +389,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,45 +564,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="447.6640625" customWidth="1"/>
-    <col min="4" max="5" width="26.6640625" customWidth="1"/>
-    <col min="7" max="10" width="20.6640625" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="4" width="1204.7109375" customWidth="1"/>
+    <col min="4" max="5" width="26.7109375" customWidth="1"/>
+    <col min="7" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="B2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="J3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -616,15 +616,13 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="J4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -634,13 +632,12 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2"/>
       <c r="J5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -648,136 +645,310 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>14</v>
+      </c>
       <c r="J6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="1"/>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="1"/>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="1"/>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="1"/>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="1"/>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="1"/>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="1"/>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1"/>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="1"/>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="1"/>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="1"/>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="1"/>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="1"/>
+      <c r="C26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="J7" t="s">
+      <c r="D26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="J8" t="s">
+      <c r="E26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
+    <row r="27" spans="2:5">
+      <c r="B27" s="1"/>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="1"/>
+      <c r="C28" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="J10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="J11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="2"/>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="H4:H14"/>
+  <mergeCells count="8">
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B0:B15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B1:B26"/>
+    <mergeCell ref="B0:B27"/>
+    <mergeCell ref="B1:B27"/>
+    <mergeCell ref="B1:B28"/>
+    <mergeCell ref="H1:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>